<commit_message>
minor changes in all files
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/BankFormData.xlsx
+++ b/src/test/resources/TestData/BankFormData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\IdeaProjects\AssetManagement\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3894FA8B-B22D-416D-AB8E-FB67AF8979EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFFD97C-0492-4458-85E3-A253632B497A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,15 +93,6 @@
     <t>WI002</t>
   </si>
   <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>California</t>
-  </si>
-  <si>
-    <t>Los Angeles</t>
-  </si>
-  <si>
     <t>Jane Smith</t>
   </si>
   <si>
@@ -114,12 +105,6 @@
     <t>WI003</t>
   </si>
   <si>
-    <t>UK</t>
-  </si>
-  <si>
-    <t>London</t>
-  </si>
-  <si>
     <t>Robert Brown</t>
   </si>
   <si>
@@ -135,15 +120,6 @@
     <t>WI004</t>
   </si>
   <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>Ontario</t>
-  </si>
-  <si>
-    <t>Toronto</t>
-  </si>
-  <si>
     <t>Alice Green</t>
   </si>
   <si>
@@ -156,15 +132,6 @@
     <t>WI005</t>
   </si>
   <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>New South Wales</t>
-  </si>
-  <si>
-    <t>Sydney</t>
-  </si>
-  <si>
     <t>Michael White</t>
   </si>
   <si>
@@ -184,13 +151,46 @@
   </si>
   <si>
     <t>C:\Users\Lenovo\IdeaProjects\AssetManagement\src\test\resources\TestData\BankLogos\logo5.png</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Berat</t>
+  </si>
+  <si>
+    <t>Ure Vajgurore</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Hidd</t>
+  </si>
+  <si>
+    <t>Haiti</t>
+  </si>
+  <si>
+    <t>Centre</t>
+  </si>
+  <si>
+    <t>Hinche</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>Midlands</t>
+  </si>
+  <si>
+    <t>Zvishavane</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +214,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFE0E4DB"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -236,7 +242,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -247,6 +253,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -528,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,7 +594,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -622,10 +629,10 @@
         <v>19</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
@@ -633,13 +640,13 @@
         <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>24</v>
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
       </c>
       <c r="F3" s="2">
         <v>34.052199999999999</v>
@@ -648,10 +655,10 @@
         <v>-118.2437</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J3" s="2">
         <v>1234567890</v>
@@ -660,24 +667,24 @@
         <v>19</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F4" s="2">
         <v>51.507399999999997</v>
@@ -686,36 +693,36 @@
         <v>-0.1278</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="J4" s="2">
         <v>2345678901</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="F5" s="2">
         <v>43.6511</v>
@@ -724,10 +731,10 @@
         <v>-79.346999999999994</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="J5" s="2">
         <v>3456789012</v>
@@ -736,24 +743,24 @@
         <v>19</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F6" s="2">
         <v>-33.8688</v>
@@ -762,20 +769,23 @@
         <v>151.20930000000001</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J6" s="2">
         <v>4567890123</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>52</v>
-      </c>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E8" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -786,5 +796,6 @@
     <hyperlink ref="I6" r:id="rId5" display="mailto:michael.white@example.com" xr:uid="{96D34ABF-2946-4AE6-9173-89250F14D4F5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>